<commit_message>
1. Add TX board command. 2. Update the script template for CAR.
</commit_message>
<xml_diff>
--- a/branches/Woodpecker_Car/Woodpecker/Woodpecker/Reference/Schedule/Woodpecker_Script Template_CAR.xlsx
+++ b/branches/Woodpecker_Car/Woodpecker/Woodpecker/Reference/Schedule/Woodpecker_Script Template_CAR.xlsx
@@ -37,10 +37,10 @@
     <definedName name="_log">List!$G$2:$G$3</definedName>
     <definedName name="_NEL" comment="在_ascii code後選擇利用\r \n \r\n \n\r換行的清單">List!$H$3:$H$6</definedName>
     <definedName name="_no" comment="選擇數字1-10的清單">List!$B$20:$B$29</definedName>
-    <definedName name="_P_cmd" comment="接收到訊號後的動作選單">List!$G$19:$G$27</definedName>
+    <definedName name="_P_cmd" comment="接收到訊號後的動作選單">List!$G$19:$G$25</definedName>
     <definedName name="_Remark">Remark!$B$2:$C$135</definedName>
     <definedName name="_temp" comment="溫度選單-20~50">List!$K$9:$K$23</definedName>
-    <definedName name="Cmd_list">List!$A$2:$A$19</definedName>
+    <definedName name="Cmd_list">List!$A$2:$A$21</definedName>
     <definedName name="COM" comment="COM PORT">List!$D$2:$D$8</definedName>
     <definedName name="Pin">List!$D$19:$D$30</definedName>
     <definedName name="switch">List!$H$13:$H$22</definedName>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="738">
   <si>
     <t>SerialPort I/O comd</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1413,6 +1413,10 @@
   </si>
   <si>
     <t>\n</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -5029,31 +5033,43 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>_savelog</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_savelog</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lens</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>ALL</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>_save</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>_savelog_</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>_mail</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>_mail</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>_savelog</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>_rc</t>
+    <t>_TX_I2C_Read</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_TX_I2C_Write</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_TX_I2C_Read</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>_TX_I2C_Write</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5428,7 +5444,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5716,6 +5732,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5726,7 +5751,434 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="74">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6124,16 +6576,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C1" s="65" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="67" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>35</v>
@@ -6145,7 +6597,7 @@
         <v>0</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="I1" s="68" t="s">
         <v>27</v>
@@ -6173,7 +6625,7 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
@@ -6185,7 +6637,7 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -6197,7 +6649,7 @@
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -6209,7 +6661,7 @@
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
@@ -6221,7 +6673,7 @@
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -6233,7 +6685,7 @@
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
@@ -6245,7 +6697,7 @@
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -6257,7 +6709,7 @@
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -6269,7 +6721,7 @@
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -6281,7 +6733,7 @@
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -6293,7 +6745,7 @@
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
@@ -6305,7 +6757,7 @@
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="G14" s="25"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
@@ -6317,7 +6769,7 @@
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="G15" s="25"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -6329,7 +6781,7 @@
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="G16" s="25"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
@@ -6341,7 +6793,7 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="G17" s="25"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
@@ -6353,7 +6805,7 @@
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18" t="str">
@@ -6368,7 +6820,7 @@
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18" t="str">
@@ -6383,7 +6835,7 @@
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18" t="str">
@@ -6398,7 +6850,7 @@
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18" t="str">
@@ -6413,7 +6865,7 @@
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18" t="str">
@@ -6428,7 +6880,7 @@
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18" t="str">
@@ -6443,7 +6895,7 @@
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="G24" s="25"/>
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18" t="str">
@@ -6458,7 +6910,7 @@
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="G25" s="25"/>
       <c r="H25" s="18"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18" t="str">
@@ -6473,7 +6925,7 @@
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="G26" s="25"/>
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18" t="str">
@@ -6488,7 +6940,7 @@
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="G27" s="25"/>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18" t="str">
@@ -6503,7 +6955,7 @@
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18" t="str">
@@ -6518,7 +6970,7 @@
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="G29" s="25"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18" t="str">
@@ -6533,7 +6985,7 @@
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="G30" s="25"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18" t="str">
@@ -6548,7 +7000,7 @@
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="G31" s="25"/>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
       <c r="J31" s="18" t="str">
@@ -6560,71 +7012,62 @@
   <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B31">
-    <cfRule type="expression" dxfId="12" priority="14">
-      <formula>IF(OR(A2="",A2="_Funckey",A2="RC Key",A2="_FuelDisplay",A2="_WaterTemp",A2="_IO_Output",A2="_IO_Input",A2="_Keyword"),0,1)</formula>
+    <cfRule type="expression" dxfId="17" priority="15">
+      <formula>IF(OR(A2="",A2="_Funckey",A2="RC Key",A2="_FuelDisplay",A2="_WaterTemp",A2="_IO_Output",A2="_IO_Input",A2="_Keyword",A2="_TX_I2C_Read"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C31">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>IF(OR(A2="",A2="_FuncKey",A2="RC Key"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D31">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>IF(OR(A2="",A2="_HEX", A2="_ascii",A2="_FuncKey",A2="_Pin"),0,1)</formula>
+    <cfRule type="expression" dxfId="15" priority="13">
+      <formula>IF(OR(A2="",A2="_HEX", A2="_ascii",A2="_FuncKey",A2="_Pin",A2="_TX_I2C_Read",A2="_TX_I2C_Write"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E31">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>IF(AND(A2="_dektec",H2="_stop"),1,0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11">
-      <formula>IF(OR(A2="",A2="_K_ABS",A2="_K_OBD", A2="_quantum",A2="_astro",A2="_dektec"),0,1)</formula>
+    <cfRule type="expression" dxfId="14" priority="12">
+      <formula>IF(OR(A2="",A2="_K_ABS",A2="_K_OBD",A2="_TX_I2C_Read",A2="_TX_I2C_Write"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="expression" dxfId="7" priority="2">
-      <formula>IF(AND(A2="_dektec",H2="_stop"),1,0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10">
-      <formula>IF(OR(A2="",A2="_quantum",A2="_dektec"),0,1)</formula>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>IF(OR(A2="",A2="_TX_I2C_Write"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="expression" dxfId="5" priority="9">
-      <formula>IF(OR(A2="_K_SEND",A2="_K_CLEAR",A2="_shot",A2="_rec_start",A2="_rec_stop",A2="_cmd",A2="_FuelDisplay",A2="_WaterTemp",A2="_IO_Output",A2="_IO_Input"),1,0)</formula>
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>IF(OR(A2="_K_SEND",A2="_K_CLEAR",A2="_shot",A2="_rec_start",A2="_rec_stop",A2="_cmd",A2="_FuelDisplay",A2="_WaterTemp",A2="_IO_Output",A2="_IO_Input",A2="_TX_I2C_Read",A2="_TX_I2C_Write"),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>IF(AND(A2="_ascii",G2="_clear"),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>IF(AND(A2="_ascii",G2="_save"),1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
-      <formula>IF(OR(A2="",A2="_ascii",A2="_FuncKey",A2="_cmd",A2="_dektec"),0,1)</formula>
+    <cfRule type="expression" dxfId="11" priority="9">
+      <formula>IF(OR(A2="",A2="_ascii",A2="_FuncKey",A2="_cmd"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations count="6">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A31">
       <formula1>Cmd_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31">
-      <formula1>IF(OR(A2="_HEX",A2="_ascii",A2="_FuncKey"),COM, IF(A2="_Pin",Pin,""))</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G31">
-      <formula1>IF(OR(A3="_HEX",A3="_ascii"),_log,IF(E3="Front tyre",_ABS_front,IF(E3="Rare tyre",_ABS_rare,IF(E3="Other",_ABS_other,IF(A3="_Temperature",_temp,IF(OR(A3="_Pin",A3="_keyword"),_P_cmd,""))))))</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H31">
       <formula1>IF(A2="_ascii",_NEL,IF(A2="_FuncKey",_NEL,IF(A2="_cmd",switch,IF(A2="_dektec",_dektec,""))))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B6:B31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B31">
       <formula1>IF(A2="_FuncKey",_no,"")</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E31">
       <formula1>INDIRECT(A2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31">
+      <formula1>IF(OR(A2="_HEX",A2="_ascii",A2="_FuncKey",A2="TX_I2C_Read",A2="TX_I2C_Write"),COM, IF(A2="_Pin",Pin,""))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6636,7 +7079,7 @@
           <x14:formula1>
             <xm:f>IF(OR(A2="_HEX",A2="_ascii"),_log, IF(E2=List!$E$13:$E$22,INDIRECT(A2),IF(A2="_Temperature",_temp,IF(A2="_Pin",_P_cmd,""))))</xm:f>
           </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
+          <xm:sqref>G2:G31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6650,7 +7093,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -6665,10 +7108,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B1" s="86" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C1" s="62" t="s">
         <v>28</v>
@@ -6680,13 +7123,13 @@
         <v>35</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="G1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>542</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>541</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>27</v>
@@ -6703,7 +7146,7 @@
         <v>36</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
@@ -6715,8 +7158,8 @@
       <c r="D3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="21"/>
+      <c r="H3" s="31" t="s">
         <v>44</v>
       </c>
       <c r="K3" s="16"/>
@@ -6724,7 +7167,7 @@
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="88" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>38</v>
@@ -6737,7 +7180,7 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>39</v>
@@ -6750,34 +7193,34 @@
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>43</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="88" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>721</v>
+        <v>733</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="88" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="88" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -6787,7 +7230,7 @@
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="88" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -6797,7 +7240,7 @@
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="88" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -6881,7 +7324,7 @@
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -6897,7 +7340,7 @@
     </row>
     <row r="18" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="88" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -6913,10 +7356,10 @@
     </row>
     <row r="19" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="88" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D19" s="92" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>302</v>
@@ -6925,16 +7368,19 @@
         <v>29</v>
       </c>
       <c r="H19" s="97" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="K19" s="20">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="90" t="s">
+        <v>734</v>
+      </c>
       <c r="B20" s="16"/>
       <c r="D20" s="93" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>303</v>
@@ -6950,9 +7396,12 @@
       </c>
     </row>
     <row r="21" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="90" t="s">
+        <v>735</v>
+      </c>
       <c r="B21" s="16"/>
       <c r="D21" s="93" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>304</v>
@@ -6961,7 +7410,7 @@
         <v>30</v>
       </c>
       <c r="H21" s="97" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="K21" s="20">
         <v>40</v>
@@ -6970,7 +7419,7 @@
     <row r="22" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
       <c r="D22" s="93" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>305</v>
@@ -6989,7 +7438,7 @@
       <c r="B23" s="16"/>
       <c r="C23"/>
       <c r="D23" s="44" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>32</v>
@@ -7003,10 +7452,10 @@
       <c r="B24" s="16"/>
       <c r="C24"/>
       <c r="D24" s="44" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>730</v>
+        <v>34</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -7014,10 +7463,10 @@
       <c r="B25" s="16"/>
       <c r="C25"/>
       <c r="D25" s="44" t="s">
-        <v>530</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>733</v>
+        <v>531</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>729</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -7025,40 +7474,35 @@
       <c r="B26" s="16"/>
       <c r="C26"/>
       <c r="D26" s="44" t="s">
-        <v>531</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>34</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="16"/>
       <c r="C27"/>
       <c r="D27" s="44" t="s">
-        <v>532</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>729</v>
+        <v>533</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="16"/>
       <c r="C28"/>
       <c r="D28" s="44" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="16"/>
       <c r="C29"/>
       <c r="D29" s="44" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30"/>
       <c r="D30" s="45" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -9010,7 +9454,7 @@
         <v>369</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>371</v>
@@ -9128,7 +9572,7 @@
         <v>386</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -9140,10 +9584,10 @@
         <v>309</v>
       </c>
       <c r="J13" s="43" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -9159,10 +9603,10 @@
         <v>318</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -9172,10 +9616,10 @@
         <v>321</v>
       </c>
       <c r="J14" s="43" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -9191,10 +9635,10 @@
         <v>330</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -9207,7 +9651,7 @@
         <v>381</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -9223,10 +9667,10 @@
         <v>341</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -9236,10 +9680,10 @@
         <v>344</v>
       </c>
       <c r="J16" s="43" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -9257,10 +9701,10 @@
         <v>307</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -9270,10 +9714,10 @@
         <v>352</v>
       </c>
       <c r="J17" s="43" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -9289,10 +9733,10 @@
         <v>319</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -9302,10 +9746,10 @@
         <v>360</v>
       </c>
       <c r="J18" s="43" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -9321,10 +9765,10 @@
         <v>331</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -9334,10 +9778,10 @@
         <v>367</v>
       </c>
       <c r="J19" s="43" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -9353,10 +9797,10 @@
         <v>342</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -9369,7 +9813,7 @@
         <v>385</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -9387,10 +9831,10 @@
         <v>308</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -9405,7 +9849,7 @@
         <v>387</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -9424,7 +9868,7 @@
         <v>380</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -9437,7 +9881,7 @@
         <v>388</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -9456,7 +9900,7 @@
         <v>383</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -9469,7 +9913,7 @@
         <v>389</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -9488,7 +9932,7 @@
         <v>382</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -9501,7 +9945,7 @@
         <v>390</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -9520,7 +9964,7 @@
         <v>384</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -9533,7 +9977,7 @@
         <v>391</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -9552,7 +9996,7 @@
         <v>392</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -9565,7 +10009,7 @@
         <v>393</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -9588,10 +10032,10 @@
         <v>368</v>
       </c>
       <c r="J27" s="43" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -9614,10 +10058,10 @@
         <v>375</v>
       </c>
       <c r="J28" s="43" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -9642,10 +10086,10 @@
         <v>311</v>
       </c>
       <c r="J29" s="43" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -9671,7 +10115,7 @@
         <v>394</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -9697,7 +10141,7 @@
         <v>395</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -9723,7 +10167,7 @@
         <v>396</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -9746,10 +10190,10 @@
         <v>354</v>
       </c>
       <c r="J33" s="43" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -9772,10 +10216,10 @@
         <v>362</v>
       </c>
       <c r="J34" s="43" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -9801,7 +10245,7 @@
         <v>397</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -9824,10 +10268,10 @@
         <v>376</v>
       </c>
       <c r="J36" s="43" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -9855,7 +10299,7 @@
         <v>398</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -9881,7 +10325,7 @@
         <v>399</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -9907,7 +10351,7 @@
         <v>400</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -9933,7 +10377,7 @@
         <v>401</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -9959,7 +10403,7 @@
         <v>402</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -9982,10 +10426,10 @@
         <v>363</v>
       </c>
       <c r="J42" s="43" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -10008,10 +10452,10 @@
         <v>370</v>
       </c>
       <c r="J43" s="43" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -10034,10 +10478,10 @@
         <v>377</v>
       </c>
       <c r="J44" s="43" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -10065,7 +10509,7 @@
         <v>403</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -10091,7 +10535,7 @@
         <v>404</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -10117,7 +10561,7 @@
         <v>405</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -10143,7 +10587,7 @@
         <v>406</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -10169,7 +10613,7 @@
         <v>407</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
@@ -10195,7 +10639,7 @@
         <v>408</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -10218,10 +10662,10 @@
         <v>371</v>
       </c>
       <c r="J51" s="43" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -10244,10 +10688,10 @@
         <v>378</v>
       </c>
       <c r="J52" s="43" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
@@ -10275,7 +10719,7 @@
         <v>409</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -10298,10 +10742,10 @@
         <v>326</v>
       </c>
       <c r="J54" s="43" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -10327,7 +10771,7 @@
         <v>410</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -10350,10 +10794,10 @@
         <v>349</v>
       </c>
       <c r="J56" s="43" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -10379,7 +10823,7 @@
         <v>411</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -10405,7 +10849,7 @@
         <v>412</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -10428,10 +10872,10 @@
         <v>372</v>
       </c>
       <c r="J59" s="43" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -10457,7 +10901,7 @@
         <v>413</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -10482,10 +10926,10 @@
         <v>315</v>
       </c>
       <c r="J61" s="43" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
@@ -10508,10 +10952,10 @@
         <v>327</v>
       </c>
       <c r="J62" s="43" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -10543,7 +10987,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C69" s="42" t="s">
         <v>386</v>
@@ -10555,7 +10999,7 @@
         <v>318</v>
       </c>
       <c r="C70" s="42" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D70" s="1"/>
     </row>
@@ -10564,7 +11008,7 @@
         <v>330</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D71" s="1"/>
     </row>
@@ -10573,7 +11017,7 @@
         <v>341</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D72" s="1"/>
     </row>
@@ -10582,7 +11026,7 @@
         <v>307</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D73" s="1"/>
     </row>
@@ -10591,7 +11035,7 @@
         <v>319</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D74" s="1"/>
     </row>
@@ -10600,7 +11044,7 @@
         <v>331</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D75" s="1"/>
     </row>
@@ -10609,7 +11053,7 @@
         <v>342</v>
       </c>
       <c r="C76" s="42" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D76" s="1"/>
     </row>
@@ -10618,7 +11062,7 @@
         <v>308</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D77" s="1"/>
     </row>
@@ -10672,7 +11116,7 @@
         <v>309</v>
       </c>
       <c r="C83" s="43" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D83" s="1"/>
     </row>
@@ -10681,7 +11125,7 @@
         <v>321</v>
       </c>
       <c r="C84" s="43" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D84" s="1"/>
     </row>
@@ -10699,7 +11143,7 @@
         <v>344</v>
       </c>
       <c r="C86" s="43" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D86" s="1"/>
     </row>
@@ -10708,7 +11152,7 @@
         <v>352</v>
       </c>
       <c r="C87" s="43" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D87" s="1"/>
     </row>
@@ -10717,7 +11161,7 @@
         <v>360</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D88" s="1"/>
     </row>
@@ -10726,7 +11170,7 @@
         <v>367</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D89" s="1"/>
     </row>
@@ -10798,7 +11242,7 @@
         <v>368</v>
       </c>
       <c r="C97" s="43" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D97" s="1"/>
     </row>
@@ -10807,7 +11251,7 @@
         <v>375</v>
       </c>
       <c r="C98" s="43" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D98" s="1"/>
     </row>
@@ -10816,7 +11260,7 @@
         <v>311</v>
       </c>
       <c r="C99" s="43" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D99" s="1"/>
     </row>
@@ -10852,7 +11296,7 @@
         <v>354</v>
       </c>
       <c r="C103" s="43" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D103" s="1"/>
     </row>
@@ -10861,7 +11305,7 @@
         <v>362</v>
       </c>
       <c r="C104" s="43" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D104" s="1"/>
     </row>
@@ -10879,7 +11323,7 @@
         <v>376</v>
       </c>
       <c r="C106" s="43" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D106" s="1"/>
     </row>
@@ -10933,16 +11377,16 @@
         <v>363</v>
       </c>
       <c r="C112" s="43" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D112" s="1"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C113" s="91" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D113" s="1"/>
     </row>
@@ -11005,7 +11449,7 @@
         <v>371</v>
       </c>
       <c r="C120" s="43" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D120" s="1"/>
     </row>
@@ -11014,7 +11458,7 @@
         <v>378</v>
       </c>
       <c r="C121" s="43" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D121" s="1"/>
     </row>
@@ -11032,7 +11476,7 @@
         <v>326</v>
       </c>
       <c r="C123" s="43" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D123" s="1"/>
     </row>
@@ -11050,7 +11494,7 @@
         <v>349</v>
       </c>
       <c r="C125" s="43" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D125" s="1"/>
     </row>
@@ -11077,7 +11521,7 @@
         <v>372</v>
       </c>
       <c r="C128" s="43" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D128" s="1"/>
     </row>
@@ -11095,7 +11539,7 @@
         <v>315</v>
       </c>
       <c r="C130" s="43" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D130" s="1"/>
     </row>
@@ -11104,7 +11548,7 @@
         <v>327</v>
       </c>
       <c r="C131" s="43" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D131" s="1"/>
     </row>
@@ -11119,7 +11563,7 @@
   <sheetPr codeName="工作表5"/>
   <dimension ref="A2:M135"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
@@ -11131,16 +11575,16 @@
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="K2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -11148,10 +11592,10 @@
         <v>54</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="K3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -11159,16 +11603,16 @@
         <v>57</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="K4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M4" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -11176,7 +11620,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -11184,10 +11628,10 @@
         <v>63</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="K6" s="84" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -11195,7 +11639,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -11203,7 +11647,7 @@
         <v>68</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -11211,7 +11655,7 @@
         <v>70</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -11235,7 +11679,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -11243,7 +11687,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -11251,7 +11695,7 @@
         <v>80</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -11259,7 +11703,7 @@
         <v>82</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -11267,7 +11711,7 @@
         <v>84</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -11275,7 +11719,7 @@
         <v>86</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -11283,7 +11727,7 @@
         <v>88</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -11291,7 +11735,7 @@
         <v>90</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -11299,7 +11743,7 @@
         <v>92</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -11307,7 +11751,7 @@
         <v>94</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -11315,7 +11759,7 @@
         <v>96</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -11323,7 +11767,7 @@
         <v>98</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -11331,7 +11775,7 @@
         <v>101</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -11339,7 +11783,7 @@
         <v>103</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -11347,7 +11791,7 @@
         <v>105</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -11355,7 +11799,7 @@
         <v>107</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -11363,7 +11807,7 @@
         <v>109</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -11371,7 +11815,7 @@
         <v>111</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -11379,7 +11823,7 @@
         <v>113</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -11387,7 +11831,7 @@
         <v>115</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -11395,7 +11839,7 @@
         <v>117</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -11403,7 +11847,7 @@
         <v>119</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -11411,7 +11855,7 @@
         <v>121</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -11419,7 +11863,7 @@
         <v>123</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -11427,7 +11871,7 @@
         <v>125</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -11435,7 +11879,7 @@
         <v>127</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
@@ -11443,7 +11887,7 @@
         <v>129</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -11451,7 +11895,7 @@
         <v>131</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -11459,7 +11903,7 @@
         <v>133</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -11467,7 +11911,7 @@
         <v>135</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -11475,7 +11919,7 @@
         <v>137</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
@@ -11483,7 +11927,7 @@
         <v>139</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -11491,7 +11935,7 @@
         <v>141</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -11499,7 +11943,7 @@
         <v>143</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
@@ -11507,7 +11951,7 @@
         <v>145</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -11515,7 +11959,7 @@
         <v>147</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
@@ -11523,7 +11967,7 @@
         <v>149</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
@@ -11531,7 +11975,7 @@
         <v>151</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
@@ -11539,7 +11983,7 @@
         <v>153</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
@@ -11547,7 +11991,7 @@
         <v>155</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
@@ -11555,7 +11999,7 @@
         <v>157</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
@@ -11563,7 +12007,7 @@
         <v>159</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
@@ -11571,7 +12015,7 @@
         <v>161</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
@@ -11579,7 +12023,7 @@
         <v>163</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
@@ -11587,7 +12031,7 @@
         <v>165</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
@@ -11595,7 +12039,7 @@
         <v>167</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
@@ -11603,7 +12047,7 @@
         <v>169</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
@@ -11611,7 +12055,7 @@
         <v>171</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
@@ -11619,7 +12063,7 @@
         <v>173</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
@@ -11627,7 +12071,7 @@
         <v>175</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
@@ -11635,7 +12079,7 @@
         <v>177</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
@@ -11643,7 +12087,7 @@
         <v>179</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
@@ -11651,7 +12095,7 @@
         <v>181</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -11659,7 +12103,7 @@
         <v>183</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -11667,7 +12111,7 @@
         <v>185</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
@@ -11675,7 +12119,7 @@
         <v>187</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -11683,7 +12127,7 @@
         <v>189</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -11691,7 +12135,7 @@
         <v>191</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
@@ -11699,7 +12143,7 @@
         <v>193</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
@@ -11707,7 +12151,7 @@
         <v>195</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
@@ -11715,7 +12159,7 @@
         <v>197</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
@@ -11723,7 +12167,7 @@
         <v>199</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
@@ -11731,7 +12175,7 @@
         <v>201</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
@@ -11739,7 +12183,7 @@
         <v>203</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
@@ -11747,7 +12191,7 @@
         <v>205</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
@@ -11755,7 +12199,7 @@
         <v>207</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
@@ -11763,7 +12207,7 @@
         <v>209</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
@@ -11771,7 +12215,7 @@
         <v>211</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
@@ -11779,7 +12223,7 @@
         <v>214</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
@@ -11787,7 +12231,7 @@
         <v>216</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
@@ -11795,7 +12239,7 @@
         <v>218</v>
       </c>
       <c r="C82" s="24" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
@@ -11803,7 +12247,7 @@
         <v>220</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
@@ -11811,7 +12255,7 @@
         <v>222</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
@@ -11819,7 +12263,7 @@
         <v>224</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
@@ -11827,7 +12271,7 @@
         <v>226</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
@@ -11835,7 +12279,7 @@
         <v>228</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
@@ -11843,7 +12287,7 @@
         <v>230</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
@@ -11851,7 +12295,7 @@
         <v>232</v>
       </c>
       <c r="C89" s="24" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
@@ -11859,7 +12303,7 @@
         <v>234</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
@@ -11867,7 +12311,7 @@
         <v>236</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
@@ -11875,7 +12319,7 @@
         <v>238</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
@@ -11883,7 +12327,7 @@
         <v>240</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
@@ -11891,7 +12335,7 @@
         <v>242</v>
       </c>
       <c r="C94" s="24" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
@@ -11899,7 +12343,7 @@
         <v>244</v>
       </c>
       <c r="C95" s="24" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
@@ -11907,7 +12351,7 @@
         <v>246</v>
       </c>
       <c r="C96" s="24" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -11915,7 +12359,7 @@
         <v>248</v>
       </c>
       <c r="C97" s="24" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
@@ -11923,7 +12367,7 @@
         <v>250</v>
       </c>
       <c r="C98" s="24" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
@@ -12107,7 +12551,7 @@
         <v>-20</v>
       </c>
       <c r="C121" s="81" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
@@ -12115,7 +12559,7 @@
         <v>-15</v>
       </c>
       <c r="C122" s="82" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
@@ -12123,7 +12567,7 @@
         <v>-10</v>
       </c>
       <c r="C123" s="82" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
@@ -12131,7 +12575,7 @@
         <v>-5</v>
       </c>
       <c r="C124" s="82" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
@@ -12139,7 +12583,7 @@
         <v>0</v>
       </c>
       <c r="C125" s="82" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
@@ -12147,7 +12591,7 @@
         <v>5</v>
       </c>
       <c r="C126" s="82" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
@@ -12155,7 +12599,7 @@
         <v>10</v>
       </c>
       <c r="C127" s="82" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
@@ -12163,7 +12607,7 @@
         <v>15</v>
       </c>
       <c r="C128" s="82" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
@@ -12171,7 +12615,7 @@
         <v>20</v>
       </c>
       <c r="C129" s="82" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
@@ -12179,7 +12623,7 @@
         <v>25</v>
       </c>
       <c r="C130" s="82" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
@@ -12187,7 +12631,7 @@
         <v>30</v>
       </c>
       <c r="C131" s="82" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
@@ -12195,7 +12639,7 @@
         <v>35</v>
       </c>
       <c r="C132" s="82" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
@@ -12203,7 +12647,7 @@
         <v>40</v>
       </c>
       <c r="C133" s="82" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
@@ -12211,7 +12655,7 @@
         <v>45</v>
       </c>
       <c r="C134" s="82" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
@@ -12219,7 +12663,7 @@
         <v>50</v>
       </c>
       <c r="C135" s="83" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -12235,8 +12679,8 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -12255,16 +12699,16 @@
   <sheetData>
     <row r="1" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C1" s="65" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="67" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>23</v>
@@ -12276,7 +12720,7 @@
         <v>0</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="I1" s="68" t="s">
         <v>27</v>
@@ -12297,7 +12741,7 @@
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="71" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E2" s="51"/>
       <c r="F2" s="51"/>
@@ -12313,13 +12757,17 @@
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="71" t="s">
-        <v>695</v>
-      </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+        <v>696</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>415</v>
+      </c>
       <c r="G3" s="52"/>
       <c r="H3" s="33" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="I3" s="52"/>
       <c r="J3" s="53"/>
@@ -12331,12 +12779,12 @@
       <c r="B4" s="54"/>
       <c r="C4" s="54"/>
       <c r="D4" s="71" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="E4" s="54"/>
       <c r="F4" s="55"/>
       <c r="G4" s="72" t="s">
-        <v>728</v>
+        <v>519</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="15"/>
@@ -12401,7 +12849,7 @@
       <c r="H8" s="56"/>
       <c r="I8" s="16"/>
       <c r="J8" s="57" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -12417,12 +12865,12 @@
       <c r="H9" s="58"/>
       <c r="I9" s="32"/>
       <c r="J9" s="59" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B10" s="54"/>
       <c r="C10" s="54"/>
@@ -12438,7 +12886,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B11" s="54"/>
       <c r="C11" s="54"/>
@@ -12452,7 +12900,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="56"/>
@@ -12466,7 +12914,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="76" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B13" s="58"/>
       <c r="C13" s="58"/>
@@ -12480,7 +12928,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="75" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B14" s="56"/>
       <c r="C14" s="56"/>
@@ -12585,7 +13033,7 @@
       <c r="F20" s="56"/>
       <c r="G20" s="56"/>
       <c r="H20" s="78" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="57"/>
@@ -12625,7 +13073,7 @@
       <c r="F22" s="56"/>
       <c r="G22" s="56"/>
       <c r="H22" s="78" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="57"/>
@@ -12658,7 +13106,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B24" s="56"/>
       <c r="C24" s="56"/>
@@ -12716,10 +13164,10 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
@@ -12737,10 +13185,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C28" s="58"/>
       <c r="D28" s="58"/>
@@ -12758,12 +13206,12 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="75" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B29" s="56"/>
       <c r="C29" s="56"/>
       <c r="D29" s="80" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E29" s="56"/>
       <c r="F29" s="56"/>
@@ -12784,7 +13232,7 @@
       <c r="B30" s="56"/>
       <c r="C30" s="56"/>
       <c r="D30" s="80" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E30" s="56"/>
       <c r="F30" s="56"/>
@@ -12805,7 +13253,7 @@
       <c r="B31" s="56"/>
       <c r="C31" s="56"/>
       <c r="D31" s="80" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E31" s="56"/>
       <c r="F31" s="56"/>
@@ -12827,7 +13275,7 @@
       <c r="B32" s="56"/>
       <c r="C32" s="56"/>
       <c r="D32" s="80" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E32" s="56"/>
       <c r="F32" s="56"/>
@@ -12848,7 +13296,7 @@
       <c r="B33" s="56"/>
       <c r="C33" s="56"/>
       <c r="D33" s="80" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E33" s="56"/>
       <c r="F33" s="56"/>
@@ -12869,12 +13317,12 @@
       <c r="B34" s="56"/>
       <c r="C34" s="56"/>
       <c r="D34" s="80" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E34" s="56"/>
       <c r="F34" s="56"/>
       <c r="G34" s="14" t="s">
-        <v>731</v>
+        <v>33</v>
       </c>
       <c r="H34" s="56"/>
       <c r="I34" s="16"/>
@@ -12891,12 +13339,12 @@
       <c r="B35" s="56"/>
       <c r="C35" s="56"/>
       <c r="D35" s="80" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E35" s="56"/>
       <c r="F35" s="56"/>
       <c r="G35" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H35" s="56"/>
       <c r="I35" s="16"/>
@@ -12912,12 +13360,12 @@
       <c r="B36" s="56"/>
       <c r="C36" s="56"/>
       <c r="D36" s="80" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E36" s="56"/>
       <c r="F36" s="56"/>
       <c r="G36" s="14" t="s">
-        <v>34</v>
+        <v>728</v>
       </c>
       <c r="H36" s="56"/>
       <c r="I36" s="16"/>
@@ -12934,13 +13382,11 @@
       <c r="B37" s="56"/>
       <c r="C37" s="56"/>
       <c r="D37" s="80" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E37" s="56"/>
       <c r="F37" s="56"/>
-      <c r="G37" s="1" t="s">
-        <v>732</v>
-      </c>
+      <c r="G37" s="1"/>
       <c r="H37" s="56"/>
       <c r="I37" s="16"/>
       <c r="J37" s="57"/>
@@ -12957,7 +13403,7 @@
       <c r="B38" s="56"/>
       <c r="C38" s="56"/>
       <c r="D38" s="80" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E38" s="56"/>
       <c r="F38" s="56"/>
@@ -12977,7 +13423,7 @@
       <c r="B39" s="56"/>
       <c r="C39" s="56"/>
       <c r="D39" s="80" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E39" s="56"/>
       <c r="F39" s="56"/>
@@ -12997,7 +13443,7 @@
       <c r="B40" s="56"/>
       <c r="C40" s="56"/>
       <c r="D40" s="80" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E40" s="56"/>
       <c r="F40" s="56"/>
@@ -13014,40 +13460,52 @@
       <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="46"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
+      <c r="A41" s="46" t="s">
+        <v>736</v>
+      </c>
+      <c r="B41" s="46" t="s">
+        <v>730</v>
+      </c>
+      <c r="C41" s="54"/>
       <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
+      <c r="E41" s="46" t="s">
+        <v>731</v>
+      </c>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
+      <c r="J41" s="100"/>
       <c r="K41" s="11"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
+      <c r="A42" s="99" t="s">
+        <v>737</v>
+      </c>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="99"/>
+      <c r="E42" s="99" t="s">
+        <v>731</v>
+      </c>
+      <c r="F42" s="99" t="s">
+        <v>732</v>
+      </c>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="99"/>
+      <c r="J42" s="101"/>
       <c r="K42" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="73" priority="2">
       <formula>IF(OR(A2="",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="72" priority="1">
       <formula>IF(OR(A2="_ascii",A2="_cmd",A2="_dektec"),0,1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13074,25 +13532,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
-        <v>543</v>
-      </c>
-      <c r="B1" s="100"/>
+      <c r="A1" s="102" t="s">
+        <v>544</v>
+      </c>
+      <c r="B1" s="103"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -13100,10 +13558,10 @@
     </row>
     <row r="4" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C4" s="40"/>
       <c r="D4" s="40"/>
@@ -13111,10 +13569,10 @@
     </row>
     <row r="5" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C5" s="40"/>
       <c r="D5" s="40"/>
@@ -13122,18 +13580,18 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C7" s="38"/>
       <c r="D7" s="38"/>
@@ -13144,10 +13602,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -13158,10 +13616,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -13172,10 +13630,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
+        <v>559</v>
+      </c>
+      <c r="B10" s="38" t="s">
         <v>558</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>557</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -13189,7 +13647,7 @@
         <v>64</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
@@ -13203,7 +13661,7 @@
         <v>55</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
@@ -13214,10 +13672,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
+        <v>562</v>
+      </c>
+      <c r="B13" s="38" t="s">
         <v>561</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>560</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
@@ -13228,10 +13686,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
@@ -13242,10 +13700,10 @@
     </row>
     <row r="15" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
@@ -13253,10 +13711,10 @@
     </row>
     <row r="16" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
@@ -13264,10 +13722,10 @@
     </row>
     <row r="17" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
@@ -13275,10 +13733,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
@@ -13289,10 +13747,10 @@
     </row>
     <row r="19" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
@@ -13303,7 +13761,7 @@
         <v>300</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
@@ -13314,7 +13772,7 @@
         <v>301</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
@@ -13325,7 +13783,7 @@
         <v>302</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C22" s="40"/>
       <c r="D22" s="40"/>
@@ -13336,7 +13794,7 @@
         <v>303</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
@@ -13347,7 +13805,7 @@
         <v>304</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
@@ -13358,7 +13816,7 @@
         <v>305</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="40"/>
@@ -13366,10 +13824,10 @@
     </row>
     <row r="26" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C26" s="40"/>
       <c r="D26" s="40"/>
@@ -13377,10 +13835,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="40"/>
@@ -13391,18 +13849,18 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="C29" s="40"/>
       <c r="D29" s="40"/>
@@ -13413,10 +13871,10 @@
     </row>
     <row r="30" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="40"/>
@@ -13427,7 +13885,7 @@
         <v>24</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="40"/>

</xml_diff>